<commit_message>
update export question info
</commit_message>
<xml_diff>
--- a/ExportTemplates/pinTemplate.xlsx
+++ b/ExportTemplates/pinTemplate.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="120" yWindow="75" windowWidth="19095" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="Pins" sheetId="1" r:id="rId1"/>
+    <sheet name="PIN" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -19,15 +19,9 @@
     <t>#</t>
   </si>
   <si>
-    <t>Online Test - Export Pin</t>
-  </si>
-  <si>
     <t>Candidate Name</t>
   </si>
   <si>
-    <t>Pin</t>
-  </si>
-  <si>
     <t>Candidate ID</t>
   </si>
   <si>
@@ -38,6 +32,12 @@
   </si>
   <si>
     <t>Start  Date:</t>
+  </si>
+  <si>
+    <t>PIN</t>
+  </si>
+  <si>
+    <t>Online Test - Export PIN</t>
   </si>
 </sst>
 </file>
@@ -123,13 +123,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,7 +432,7 @@
   <dimension ref="B1:F8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -447,34 +447,34 @@
   <sheetData>
     <row r="1" spans="2:6" ht="11.25" customHeight="1"/>
     <row r="2" spans="2:6" ht="13.5" customHeight="1">
-      <c r="B2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="B2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="2:6" ht="21.75" customHeight="1">
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="2:6" ht="12.75" customHeight="1"/>
     <row r="5" spans="2:6" ht="12.75" customHeight="1">
-      <c r="B5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7"/>
+      <c r="B5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="2:6" ht="12.75" customHeight="1">
       <c r="B6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="2:6" ht="12.75" customHeight="1">
       <c r="B7" s="4"/>
@@ -484,16 +484,16 @@
         <v>0</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Export pin header for each candiate
</commit_message>
<xml_diff>
--- a/ExportTemplates/pinTemplate.xlsx
+++ b/ExportTemplates/pinTemplate.xlsx
@@ -432,7 +432,7 @@
   <dimension ref="B1:F8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -442,7 +442,7 @@
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
     <col min="4" max="4" width="32.5703125" customWidth="1"/>
     <col min="5" max="5" width="34.42578125" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="11.25" customHeight="1"/>

</xml_diff>

<commit_message>
update export pin format
</commit_message>
<xml_diff>
--- a/ExportTemplates/pinTemplate.xlsx
+++ b/ExportTemplates/pinTemplate.xlsx
@@ -109,7 +109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -124,6 +124,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -432,7 +435,7 @@
   <dimension ref="B1:F8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -446,38 +449,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="11.25" customHeight="1"/>
-    <row r="2" spans="2:6" ht="13.5" customHeight="1">
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="2:6" ht="29.25" customHeight="1">
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="2:6" ht="21.75" customHeight="1">
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+    <row r="3" spans="2:6" ht="12.75" customHeight="1"/>
+    <row r="4" spans="2:6" ht="12.75" customHeight="1">
+      <c r="B4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="5"/>
     </row>
-    <row r="4" spans="2:6" ht="12.75" customHeight="1"/>
     <row r="5" spans="2:6" ht="12.75" customHeight="1">
-      <c r="B5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="7"/>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="2:6" ht="12.75" customHeight="1">
-      <c r="B6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="5"/>
+      <c r="B6" s="4"/>
     </row>
     <row r="7" spans="2:6" ht="12.75" customHeight="1">
-      <c r="B7" s="4"/>
+      <c r="B7" s="6"/>
     </row>
     <row r="8" spans="2:6" s="3" customFormat="1" ht="25.5" customHeight="1">
       <c r="B8" s="2" t="s">
@@ -498,8 +497,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:F3"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>